<commit_message>
Tried to implement the psychtoolbox method of rendering the grating but rolled back to the previous method. Slight modifications in the format. Tested speed and stimulus size and spatial frequency.
</commit_message>
<xml_diff>
--- a/cond01.xlsx
+++ b/cond01.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-20" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="cond01.csv" sheetId="1" r:id="rId1"/>
@@ -452,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:I17"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -528,16 +528,16 @@
         <v>500</v>
       </c>
       <c r="F2">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G2">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>5</v>
@@ -581,16 +581,16 @@
         <v>500</v>
       </c>
       <c r="F3">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G3">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>5</v>
@@ -634,16 +634,16 @@
         <v>500</v>
       </c>
       <c r="F4">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G4">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>5</v>
@@ -687,16 +687,16 @@
         <v>500</v>
       </c>
       <c r="F5">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G5">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>5</v>
@@ -740,16 +740,16 @@
         <v>500</v>
       </c>
       <c r="F6">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J6">
         <v>5</v>
@@ -793,16 +793,16 @@
         <v>500</v>
       </c>
       <c r="F7">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G7">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I7">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>5</v>
@@ -846,16 +846,16 @@
         <v>500</v>
       </c>
       <c r="F8">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <v>5</v>
@@ -899,16 +899,16 @@
         <v>500</v>
       </c>
       <c r="F9">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G9">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I9">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>5</v>
@@ -952,16 +952,16 @@
         <v>500</v>
       </c>
       <c r="F10">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G10">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I10">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>5</v>
@@ -1005,16 +1005,16 @@
         <v>500</v>
       </c>
       <c r="F11">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G11">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I11">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <v>5</v>
@@ -1058,16 +1058,16 @@
         <v>500</v>
       </c>
       <c r="F12">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G12">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I12">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J12">
         <v>5</v>
@@ -1111,16 +1111,16 @@
         <v>500</v>
       </c>
       <c r="F13">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G13">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>5</v>
@@ -1164,16 +1164,16 @@
         <v>500</v>
       </c>
       <c r="F14">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G14">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>5</v>
@@ -1217,16 +1217,16 @@
         <v>500</v>
       </c>
       <c r="F15">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G15">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>5</v>
@@ -1270,16 +1270,16 @@
         <v>500</v>
       </c>
       <c r="F16">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H16">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I16">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J16">
         <v>5</v>
@@ -1323,16 +1323,16 @@
         <v>500</v>
       </c>
       <c r="F17">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="G17">
-        <v>6.7</v>
+        <v>4</v>
       </c>
       <c r="H17">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="I17">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="J17">
         <v>5</v>

</xml_diff>